<commit_message>
fix: throw an exception for missing fields
Missing headers had defaulted to the last+1 cell in a row.
The intention was clearly to throw an exception.

A new constructor parameter allows existing behaviour.

fix: Return meaningful errors

File Validation errors were being swallowed by incorrect use of loggers.

chore: improve code style conformance

TIS21-7129: Use Person ID to create a placement against
</commit_message>
<xml_diff>
--- a/generic-upload-service/src/test/resources/com/transformuk/hee/tis/genericupload/service/parser/XlsNotLongTestData.xlsx
+++ b/generic-upload-service/src/test/resources/com/transformuk/hee/tis/genericupload/service/parser/XlsNotLongTestData.xlsx
@@ -20,21 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve">myLong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myString</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myFloat</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myDate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">myLocalDate</t>
   </si>
   <si>
     <t xml:space="preserve"> 1.2 </t>
@@ -120,7 +108,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -130,10 +118,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -218,45 +202,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IV3"/>
+  <dimension ref="A1:IR3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="1" width="15.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="20.55"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="24.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="15.36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="9" style="1" width="18.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="28.11"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="8.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="21.73"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="14" style="1" width="11.81"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="1" width="21.26"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="1" width="19.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="1" width="23.5"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="1" width="12.4"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="256" min="20" style="1" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="1" width="15.36"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="1" width="18.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="28.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="21.73"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="10" style="1" width="11.81"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="21.26"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="19.63"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="23.5"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="1" width="12.4"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="252" min="16" style="1" width="8.74"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1021" style="0" width="10.08"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -514,14 +486,10 @@
       <c r="IP2" s="0"/>
       <c r="IQ2" s="0"/>
       <c r="IR2" s="0"/>
-      <c r="IS2" s="0"/>
-      <c r="IT2" s="0"/>
-      <c r="IU2" s="0"/>
-      <c r="IV2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>5</v>
+      <c r="A3" s="3" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>